<commit_message>
correcion base de datos
</commit_message>
<xml_diff>
--- a/Datos/Defunciones-mortalidad-materna-2011.xlsx
+++ b/Datos/Defunciones-mortalidad-materna-2011.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ponyta\Desktop\U onlain\Semestre 6\Para LET\mortalidad-materna\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3C97E63-315F-4F6A-B2C4-D7D9FFB6E0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21FC6C6A-C1AB-42EF-9818-428D4BF22FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13065" yWindow="555" windowWidth="15660" windowHeight="14070" xr2:uid="{50E56D6C-C8F5-450D-9EDA-6A15DC80C714}"/>
+    <workbookView xWindow="15" yWindow="45" windowWidth="13800" windowHeight="15630" xr2:uid="{50E56D6C-C8F5-450D-9EDA-6A15DC80C714}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,20 +34,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Aborto</t>
   </si>
   <si>
-    <t>Edema, proteinuria y trastornos hipertensivos en el embarazo, parto y el puerperio</t>
-  </si>
-  <si>
     <t>Hemorragia en el embarazo, parto y el puerperio</t>
   </si>
   <si>
-    <t>Complicaciones predominantes, relacionadas con el embarazo y el parto</t>
-  </si>
-  <si>
     <t>Sepsis puerperal y otras infecciones</t>
   </si>
   <si>
@@ -57,9 +51,6 @@
     <t>Muertes obstétricas de causa no específica</t>
   </si>
   <si>
-    <t>Muerte materna debida a cualquier causa obstétrica que ocurre después de 42 días pero antes de un año del parto</t>
-  </si>
-  <si>
     <t>Muertes obstétricas indirectas</t>
   </si>
   <si>
@@ -72,7 +63,13 @@
     <t>RMM</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>Edema, proteinuria y trastornos hipertensivos</t>
+  </si>
+  <si>
+    <t>Complicaciones predominantes</t>
+  </si>
+  <si>
+    <t>Cualquier causa obstétrica que ocurre después de 42 días pero antes de un año del parto</t>
   </si>
 </sst>
 </file>
@@ -448,23 +445,24 @@
   <dimension ref="B3:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="12" customWidth="1"/>
+    <col min="2" max="2" width="59.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.25">
@@ -480,7 +478,7 @@
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>14</v>
@@ -491,7 +489,7 @@
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -502,7 +500,7 @@
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
@@ -513,18 +511,18 @@
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>12</v>
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C9" s="1">
         <v>3</v>
@@ -535,18 +533,18 @@
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>12</v>
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C11" s="1">
         <v>6</v>
@@ -557,7 +555,7 @@
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1">
         <v>12</v>

</xml_diff>